<commit_message>
roteiro modal de opcionais
</commit_message>
<xml_diff>
--- a/TerceiroPasso/SelecaoDeOfertas.xlsx
+++ b/TerceiroPasso/SelecaoDeOfertas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTI DIGITAL\Desktop\DTI Digital\roteirosDeTeste\TerceiroPasso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E7ECD9-A1BC-47B4-9BE7-95C77C65AEBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F8A1FA-BB5D-4823-B4AC-BF95A4F06CAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="139">
   <si>
     <t>CHECKLIST FLOW</t>
   </si>
@@ -423,12 +423,6 @@
     <t>iremos exibir "Mínimo x diárias" antes do nome da oferta;</t>
   </si>
   <si>
-    <t>Caso tiver km extra ou km controlado</t>
-  </si>
-  <si>
-    <t>No caso do KM controlado é exibido "R$ x,xx por KM extra" e em caso de KM rodado é exibido "R$ x,xx por KM". O mesmo deverá ser informado (caso houver) logo abaixo do preço da oferta.</t>
-  </si>
-  <si>
     <t>Caso for tarifa selecionada</t>
   </si>
   <si>
@@ -439,6 +433,140 @@
   </si>
   <si>
     <t>A mesma deverá já vim selecionada</t>
+  </si>
+  <si>
+    <t>Km controlado</t>
+  </si>
+  <si>
+    <t>1dez 5jan Várias ofertas</t>
+  </si>
+  <si>
+    <t>2 out 9out</t>
+  </si>
+  <si>
+    <t>3out 31out confins</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se a oferta for com </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>km controlado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> e o valor por km rodado for positivo, então deve mostrar o texto: '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Valor do Km extra'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + ('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>por KM extra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">' se </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>franquia km diaria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; 0 OU '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>por KM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>' franquia km diaria &lt;= 0)</t>
+    </r>
+  </si>
+  <si>
+    <t>Falta o valor de franquia de km por diária</t>
+  </si>
+  <si>
+    <t>Falta separação da informação da descrição da oferta</t>
+  </si>
+  <si>
+    <t>Erro</t>
   </si>
 </sst>
 </file>
@@ -448,7 +576,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -577,6 +705,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -913,50 +1053,6 @@
   </cellStyleXfs>
   <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1113,11 +1209,58 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1146,9 +1289,6 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1164,6 +1304,214 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFC3924"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFC3924"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -1242,6 +1590,84 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFC3924"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -1320,6 +1746,84 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF66"/>
         </patternFill>
       </fill>
@@ -1944,6 +2448,58 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF66"/>
         </patternFill>
       </fill>
@@ -2022,6 +2578,32 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -3010,6 +3592,32 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -3062,6 +3670,84 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF66"/>
         </patternFill>
       </fill>
@@ -3479,552 +4165,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFC3924"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFC3924"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFC3924"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -7265,223 +7405,223 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="16" customWidth="1"/>
-    <col min="3" max="4" width="18.85546875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="16" customWidth="1"/>
-    <col min="6" max="18" width="9.140625" style="15" customWidth="1"/>
-    <col min="19" max="255" width="9.140625" style="16" customWidth="1"/>
-    <col min="256" max="256" width="22.5703125" style="16" customWidth="1"/>
-    <col min="257" max="1025" width="24.140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="18.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="2" customWidth="1"/>
+    <col min="6" max="18" width="9.140625" style="1" customWidth="1"/>
+    <col min="19" max="255" width="9.140625" style="2" customWidth="1"/>
+    <col min="256" max="256" width="22.5703125" style="2" customWidth="1"/>
+    <col min="257" max="1025" width="24.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:18" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+    <row r="1" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:18" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="2:18" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+    </row>
+    <row r="4" spans="2:18" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+    <row r="5" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
+      <c r="E11" s="7"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
+      <c r="E12" s="7"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
+      <c r="E13" s="7"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
+      <c r="E14" s="7"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="21"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
+      <c r="E15" s="7"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
+      <c r="E16" s="7"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-    </row>
-    <row r="18" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="E17" s="7"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:E3"/>
@@ -7522,202 +7662,215 @@
   </sheetPr>
   <dimension ref="A2:AMK12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="22" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="22" customWidth="1"/>
-    <col min="7" max="254" width="9.140625" style="22" customWidth="1"/>
-    <col min="255" max="1025" width="4" style="22" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="8" customWidth="1"/>
+    <col min="7" max="254" width="9.140625" style="8" customWidth="1"/>
+    <col min="255" max="1025" width="4" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="66"/>
+      <c r="D4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="F4" s="67"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>1</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:9" ht="90" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27" t="s">
+      <c r="F7" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C11" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F11" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="87" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="87" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>24</v>
+      <c r="F12" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -8102,101 +8255,101 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:F12">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="2" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="3" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:F12">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="4" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="5" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="6" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:F12">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="8" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="9" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="11" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="12" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="13" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="14" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="15" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="17" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="18" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="19" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="20" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="21" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="5" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="22" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="23" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="24" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="2" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="25" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="26" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="27" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8228,281 +8381,281 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="93" style="16" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="16" customWidth="1"/>
-    <col min="5" max="17" width="9.140625" style="15" customWidth="1"/>
-    <col min="18" max="254" width="9.140625" style="16" customWidth="1"/>
-    <col min="255" max="255" width="22.5703125" style="16" customWidth="1"/>
-    <col min="256" max="1025" width="24.140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="93" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
+    <col min="5" max="17" width="9.140625" style="1" customWidth="1"/>
+    <col min="18" max="254" width="9.140625" style="2" customWidth="1"/>
+    <col min="255" max="255" width="22.5703125" style="2" customWidth="1"/>
+    <col min="256" max="1025" width="24.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
     </row>
     <row r="3" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="33" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="33" t="s">
+      <c r="B8" s="70"/>
+      <c r="C8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="70"/>
+      <c r="C9" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="33" t="s">
+      <c r="B10" s="70"/>
+      <c r="C10" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="70"/>
+      <c r="C11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="2:4" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="33" t="s">
+      <c r="B14" s="68"/>
+      <c r="C14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="33" t="s">
+      <c r="B15" s="68"/>
+      <c r="C15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="68"/>
+      <c r="C16" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="68"/>
+      <c r="C17" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="31" t="s">
+      <c r="B18" s="68"/>
+      <c r="C18" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="31" t="s">
+      <c r="B19" s="68"/>
+      <c r="C19" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="33" t="s">
+      <c r="B20" s="68"/>
+      <c r="C20" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="33" t="s">
+      <c r="B23" s="68"/>
+      <c r="C23" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="33" t="s">
+      <c r="B24" s="68"/>
+      <c r="C24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="33" t="s">
+      <c r="B27" s="68"/>
+      <c r="C27" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="33" t="s">
+      <c r="B28" s="68"/>
+      <c r="C28" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:4" s="15" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+    <row r="29" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:4" s="1" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="35" t="s">
+      <c r="C33" s="69"/>
+      <c r="D33" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B22:B24"/>
@@ -8515,164 +8668,164 @@
     <mergeCell ref="B13:B20"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D6:D11 D13 D18">
-    <cfRule type="cellIs" dxfId="114" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="4" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="111" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="6" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="7" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="108" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="105" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="11" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="12" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="13" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="102" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="15" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="16" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="99" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="17" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="18" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="19" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="96" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="20" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="21" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D4">
-    <cfRule type="cellIs" dxfId="93" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="23" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="24" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="25" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="cellIs" dxfId="90" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="26" operator="equal">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="27" operator="equal">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="88" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="29" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="cellIs" dxfId="85" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="31" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="32" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="33" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="82" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="34" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="35" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="36" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="79" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="37" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="38" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="39" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="76" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="40" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="41" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="42" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="73" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8700,411 +8853,411 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="22" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="87.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="36" customWidth="1"/>
-    <col min="6" max="19" width="9.140625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="22" customWidth="1"/>
+    <col min="6" max="19" width="9.140625" style="22" customWidth="1"/>
     <col min="20" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="38"/>
+    <row r="1" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
+      <c r="B4" s="72"/>
       <c r="C4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="41" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="41" t="s">
+      <c r="B6" s="72"/>
+      <c r="C6" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="41" t="s">
+      <c r="B9" s="77"/>
+      <c r="C9" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="41" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="41" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="41" t="s">
+      <c r="B12" s="77"/>
+      <c r="C12" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="41" t="s">
+      <c r="B13" s="77"/>
+      <c r="C13" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
+    <row r="14" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="44"/>
+      <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="41" t="s">
+      <c r="B16" s="72"/>
+      <c r="C16" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="45" t="s">
+      <c r="B19" s="72"/>
+      <c r="C19" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="44"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="49" t="s">
+      <c r="B22" s="72"/>
+      <c r="C22" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="49" t="s">
+      <c r="B23" s="72"/>
+      <c r="C23" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
     </row>
     <row r="27" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="77"/>
-      <c r="D27" s="53" t="s">
+      <c r="C27" s="74"/>
+      <c r="D27" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="38"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="24"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="38"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:D13 D18:D19 D3:D6 D15:D16">
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D6 D15:D16">
-    <cfRule type="cellIs" dxfId="65" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D13">
-    <cfRule type="cellIs" dxfId="62" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D19">
-    <cfRule type="cellIs" dxfId="59" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="14" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="15" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D13">
-    <cfRule type="cellIs" dxfId="56" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D19">
-    <cfRule type="cellIs" dxfId="53" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D22">
-    <cfRule type="cellIs" dxfId="50" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D22">
-    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D22">
-    <cfRule type="cellIs" dxfId="44" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="28" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="29" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="30" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="31" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="32" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="33" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="34" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="35" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="36" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="37" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="38" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="39" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9136,10 +9289,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="36" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="36" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" style="36" customWidth="1"/>
-    <col min="4" max="1025" width="9.140625" style="36" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" style="22" customWidth="1"/>
+    <col min="4" max="1025" width="9.140625" style="22" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -9161,375 +9314,375 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="16" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="6" style="16" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="21" style="15" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="15" customWidth="1"/>
-    <col min="9" max="11" width="9.140625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="100.5703125" style="15" customWidth="1"/>
-    <col min="13" max="19" width="9.140625" style="15" customWidth="1"/>
-    <col min="20" max="256" width="9.140625" style="16" customWidth="1"/>
-    <col min="257" max="257" width="22.5703125" style="16" customWidth="1"/>
-    <col min="258" max="1025" width="24.140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="100.5703125" style="1" customWidth="1"/>
+    <col min="13" max="19" width="9.140625" style="1" customWidth="1"/>
+    <col min="20" max="256" width="9.140625" style="2" customWidth="1"/>
+    <col min="257" max="257" width="22.5703125" style="2" customWidth="1"/>
+    <col min="258" max="1025" width="24.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="36"/>
-    </row>
-    <row r="2" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="36"/>
-    </row>
-    <row r="3" spans="2:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78" t="s">
+    <row r="1" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="I3" s="79" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="I3" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-    </row>
-    <row r="4" spans="2:12" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+    </row>
+    <row r="4" spans="2:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-    </row>
-    <row r="5" spans="2:12" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="80" t="s">
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+    </row>
+    <row r="5" spans="2:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="44">
         <v>0</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="44">
         <v>2</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="45">
         <f>IF(E5&gt;D5,0,1)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="81">
+      <c r="G5" s="82">
         <v>43375</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-    </row>
-    <row r="6" spans="2:12" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="80"/>
-      <c r="C6" s="60" t="s">
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+    </row>
+    <row r="6" spans="2:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="81"/>
+      <c r="C6" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="47">
         <v>0</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="47">
         <v>0</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="48">
         <f>IF(E6&gt;D6,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="81"/>
-    </row>
-    <row r="7" spans="2:12" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="80"/>
-      <c r="C7" s="60" t="s">
+      <c r="G6" s="82"/>
+    </row>
+    <row r="7" spans="2:12" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="81"/>
+      <c r="C7" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="47">
         <v>33</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="47">
         <v>33</v>
       </c>
-      <c r="F7" s="62">
+      <c r="F7" s="48">
         <f>IF(E7&gt;D7,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G7" s="81"/>
-      <c r="I7" s="82" t="s">
+      <c r="G7" s="82"/>
+      <c r="I7" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-    </row>
-    <row r="8" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="80"/>
-      <c r="C8" s="60" t="s">
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+    </row>
+    <row r="8" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="81"/>
+      <c r="C8" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="49">
         <v>0.2</v>
       </c>
-      <c r="E8" s="63">
+      <c r="E8" s="49">
         <v>0.1</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="48">
         <f>IF(E8&lt;D8,0,1)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="81"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-    </row>
-    <row r="9" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="80"/>
-      <c r="C9" s="60" t="s">
+      <c r="G8" s="82"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+    </row>
+    <row r="9" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="81"/>
+      <c r="C9" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="49">
         <v>0.02</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="49">
         <v>0.02</v>
       </c>
-      <c r="F9" s="62">
+      <c r="F9" s="48">
         <f>IF(E9&gt;D9,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="81"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-    </row>
-    <row r="10" spans="2:12" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="83"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="84"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-    </row>
-    <row r="11" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="83"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="84"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-    </row>
-    <row r="12" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="83"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="84"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-    </row>
-    <row r="13" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="83"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="84"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-    </row>
-    <row r="14" spans="2:12" s="15" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="83"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="84"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-    </row>
-    <row r="15" spans="2:12" s="15" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="78" t="s">
+      <c r="G9" s="82"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+    </row>
+    <row r="10" spans="2:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="84"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="85"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+    </row>
+    <row r="11" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="84"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="85"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="83"/>
+    </row>
+    <row r="12" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="84"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="85"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+    </row>
+    <row r="13" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="84"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="85"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+    </row>
+    <row r="14" spans="2:12" s="1" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="84"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="85"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="83"/>
+    </row>
+    <row r="15" spans="2:12" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
-    </row>
-    <row r="16" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="69" t="s">
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
+      <c r="L15" s="83"/>
+    </row>
+    <row r="16" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="70" t="s">
+      <c r="C16" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="70" t="s">
+      <c r="F16" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="71" t="s">
+      <c r="G16" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-    </row>
-    <row r="17" spans="2:12" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="85" t="s">
+      <c r="I16" s="83"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
+    </row>
+    <row r="17" spans="2:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="61">
+      <c r="D17" s="47">
         <v>0</v>
       </c>
-      <c r="E17" s="61">
+      <c r="E17" s="47">
         <v>2</v>
       </c>
-      <c r="F17" s="61">
+      <c r="F17" s="47">
         <f>IF(E17&gt;D17,0,1)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="86">
+      <c r="G17" s="87">
         <v>43375</v>
       </c>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-    </row>
-    <row r="18" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="85"/>
-      <c r="C18" s="72" t="s">
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+    </row>
+    <row r="18" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="86"/>
+      <c r="C18" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="73">
+      <c r="D18" s="59">
         <v>0</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="59">
         <v>0</v>
       </c>
-      <c r="F18" s="73">
+      <c r="F18" s="59">
         <f>IF(E18&gt;D18,0,1)</f>
         <v>1</v>
       </c>
-      <c r="G18" s="86"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-    </row>
-    <row r="19" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="66"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
-    </row>
-    <row r="20" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="G18" s="87"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="83"/>
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+    </row>
+    <row r="19" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="52"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+    </row>
+    <row r="20" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B3:G3"/>
@@ -9544,24 +9697,24 @@
     <mergeCell ref="G17:G18"/>
   </mergeCells>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9627,13 +9780,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="61" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>